<commit_message>
Análisis combinatorio pt. 1
</commit_message>
<xml_diff>
--- a/Asistencia/AsistenciaMonitoriaED_2021_1_EnriqueNiebles.xlsx
+++ b/Asistencia/AsistenciaMonitoriaED_2021_1_EnriqueNiebles.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Enrique Niebles\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Enrique Niebles\Documents\Universidad del Norte\Ingeniería Electrónica - Sistemas y Computación\7. Séptimo Semestre\Monitoria Estructuras Discretas\Material\Asistencia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AC27180-4426-4319-B0D7-328BF1FBB6F0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{80FE9B9F-D2B4-4808-B969-05006414870B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1068" yWindow="-108" windowWidth="22080" windowHeight="13176" activeTab="1" xr2:uid="{9F616065-CB98-49F1-BECD-2AD80A2EEE2C}"/>
+    <workbookView xWindow="1068" yWindow="-108" windowWidth="22080" windowHeight="13176" xr2:uid="{9F616065-CB98-49F1-BECD-2AD80A2EEE2C}"/>
   </bookViews>
   <sheets>
     <sheet name="Asistencia" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="103">
   <si>
     <t>Estudiante</t>
   </si>
@@ -299,13 +299,58 @@
   </si>
   <si>
     <t>https://drive.google.com/file/d/1eCp0I-5bnR_u6kOsO9EofJ2_vdrJYjSy/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>Camilo Andres Cespedes</t>
+  </si>
+  <si>
+    <t>German David Vargas Ramos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Solución dudas Proyecto Computacional pt.2 </t>
+  </si>
+  <si>
+    <t>Se respondieron dudas que tenían los tutandos acerca de su proyecto computacional. No se realizó ningún nuevo ejercicio.</t>
+  </si>
+  <si>
+    <t>cacespedes</t>
+  </si>
+  <si>
+    <t>gdvargas</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1W9mYsJYUd0cGce89pEiFiieglpbeCU_8/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>Análisis combinatorio pt.1</t>
+  </si>
+  <si>
+    <t>Se introdujo el tema de análisis combinatorio, así como la solución de ejercicios utilizando funciones generadoras. Se enseñó un método para comprobar sus resultados utilizando Python.</t>
+  </si>
+  <si>
+    <t>Miguel Angel Marsiglia Arroyo</t>
+  </si>
+  <si>
+    <t>Isabella Andrea Cuesta Niebles</t>
+  </si>
+  <si>
+    <t>Vanessa Fontalvo Reniz</t>
+  </si>
+  <si>
+    <t>cuestai</t>
+  </si>
+  <si>
+    <t>mamarsiglia</t>
+  </si>
+  <si>
+    <t>vreniz</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -406,6 +451,12 @@
     <font>
       <sz val="10"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -851,10 +902,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23B5D081-BD4A-44D4-A2DC-90E7E1D86DF5}">
-  <dimension ref="B2:BB25"/>
+  <dimension ref="B2:BB30"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="V29" sqref="V29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -864,11 +915,12 @@
     <col min="3" max="3" width="38.19921875" style="2" customWidth="1"/>
     <col min="4" max="4" width="14.09765625" style="1" customWidth="1"/>
     <col min="5" max="5" width="19.19921875" style="1" customWidth="1"/>
-    <col min="6" max="19" width="11.19921875" style="1" customWidth="1"/>
-    <col min="20" max="54" width="11.19921875" style="1"/>
+    <col min="6" max="19" width="11.19921875" style="1" hidden="1" customWidth="1"/>
+    <col min="20" max="21" width="0" style="1" hidden="1" customWidth="1"/>
+    <col min="22" max="54" width="11.19921875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:20" ht="18" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:22" ht="18" x14ac:dyDescent="0.3">
       <c r="B2" s="3"/>
       <c r="C2" s="4" t="s">
         <v>0</v>
@@ -924,8 +976,14 @@
       <c r="T2" s="9">
         <v>44281</v>
       </c>
-    </row>
-    <row r="3" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="U2" s="9">
+        <v>44282</v>
+      </c>
+      <c r="V2" s="9">
+        <v>44295</v>
+      </c>
+    </row>
+    <row r="3" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B3" s="5">
         <v>1</v>
       </c>
@@ -961,8 +1019,14 @@
       <c r="T3" s="10" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="4" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="U3" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="V3" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B4" s="5">
         <v>2</v>
       </c>
@@ -992,8 +1056,10 @@
       <c r="R4" s="10"/>
       <c r="S4" s="10"/>
       <c r="T4" s="10"/>
-    </row>
-    <row r="5" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="U4" s="10"/>
+      <c r="V4" s="10"/>
+    </row>
+    <row r="5" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B5" s="5">
         <v>3</v>
       </c>
@@ -1023,24 +1089,24 @@
       <c r="T5" s="10" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="6" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="U5" s="10"/>
+      <c r="V5" s="10"/>
+    </row>
+    <row r="6" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B6" s="5">
         <v>4</v>
       </c>
-      <c r="C6" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="6">
-        <v>200128455</v>
+      <c r="C6" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="D6" s="7">
+        <v>200137946</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>30</v>
+        <v>92</v>
       </c>
       <c r="F6" s="10"/>
-      <c r="G6" s="10" t="s">
-        <v>39</v>
-      </c>
+      <c r="G6" s="10"/>
       <c r="H6" s="10"/>
       <c r="I6" s="10"/>
       <c r="J6" s="10"/>
@@ -1051,29 +1117,31 @@
       <c r="O6" s="10"/>
       <c r="P6" s="10"/>
       <c r="Q6" s="10"/>
-      <c r="R6" s="10" t="s">
-        <v>39</v>
-      </c>
+      <c r="R6" s="10"/>
       <c r="S6" s="10"/>
-      <c r="T6" s="10" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="T6" s="10"/>
+      <c r="U6" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="V6" s="10"/>
+    </row>
+    <row r="7" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B7" s="5">
         <v>5</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="7">
-        <v>200123360</v>
+        <v>4</v>
+      </c>
+      <c r="D7" s="6">
+        <v>200128455</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
+      <c r="G7" s="10" t="s">
+        <v>39</v>
+      </c>
       <c r="H7" s="10"/>
       <c r="I7" s="10"/>
       <c r="J7" s="10"/>
@@ -1082,9 +1150,7 @@
       <c r="M7" s="10"/>
       <c r="N7" s="10"/>
       <c r="O7" s="10"/>
-      <c r="P7" s="10" t="s">
-        <v>39</v>
-      </c>
+      <c r="P7" s="10"/>
       <c r="Q7" s="10"/>
       <c r="R7" s="10" t="s">
         <v>39</v>
@@ -1093,125 +1159,143 @@
       <c r="T7" s="10" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="8" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="U7" s="10"/>
+      <c r="V7" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B8" s="5">
         <v>6</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="6">
-        <v>200138598</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>32</v>
+        <v>5</v>
+      </c>
+      <c r="D8" s="7">
+        <v>200123360</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>31</v>
       </c>
       <c r="F8" s="10"/>
       <c r="G8" s="10"/>
       <c r="H8" s="10"/>
-      <c r="I8" s="10" t="s">
-        <v>39</v>
-      </c>
+      <c r="I8" s="10"/>
       <c r="J8" s="10"/>
-      <c r="K8" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="L8" s="10" t="s">
-        <v>39</v>
-      </c>
+      <c r="K8" s="10"/>
+      <c r="L8" s="10"/>
       <c r="M8" s="10"/>
       <c r="N8" s="10"/>
       <c r="O8" s="10"/>
-      <c r="P8" s="10"/>
+      <c r="P8" s="10" t="s">
+        <v>39</v>
+      </c>
       <c r="Q8" s="10"/>
-      <c r="R8" s="10"/>
+      <c r="R8" s="10" t="s">
+        <v>39</v>
+      </c>
       <c r="S8" s="10"/>
       <c r="T8" s="10" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="9" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="U8" s="10"/>
+      <c r="V8" s="10"/>
+    </row>
+    <row r="9" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B9" s="5">
         <v>7</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" s="7">
-        <v>200085471</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>33</v>
+        <v>6</v>
+      </c>
+      <c r="D9" s="6">
+        <v>200138598</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>32</v>
       </c>
       <c r="F9" s="10"/>
       <c r="G9" s="10"/>
       <c r="H9" s="10"/>
-      <c r="I9" s="10"/>
+      <c r="I9" s="10" t="s">
+        <v>39</v>
+      </c>
       <c r="J9" s="10"/>
       <c r="K9" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="L9" s="10"/>
+      <c r="L9" s="10" t="s">
+        <v>39</v>
+      </c>
       <c r="M9" s="10"/>
       <c r="N9" s="10"/>
       <c r="O9" s="10"/>
       <c r="P9" s="10"/>
       <c r="Q9" s="10"/>
-      <c r="R9" s="10" t="s">
-        <v>39</v>
-      </c>
+      <c r="R9" s="10"/>
       <c r="S9" s="10"/>
-      <c r="T9" s="10"/>
-    </row>
-    <row r="10" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="T9" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="U9" s="10"/>
+      <c r="V9" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B10" s="5">
         <v>8</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" s="6">
-        <v>200137313</v>
+        <v>7</v>
+      </c>
+      <c r="D10" s="7">
+        <v>200085471</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F10" s="10"/>
-      <c r="G10" s="10" t="s">
-        <v>39</v>
-      </c>
+      <c r="G10" s="10"/>
       <c r="H10" s="10"/>
       <c r="I10" s="10"/>
       <c r="J10" s="10"/>
-      <c r="K10" s="10"/>
+      <c r="K10" s="10" t="s">
+        <v>39</v>
+      </c>
       <c r="L10" s="10"/>
       <c r="M10" s="10"/>
       <c r="N10" s="10"/>
       <c r="O10" s="10"/>
       <c r="P10" s="10"/>
-      <c r="Q10" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="R10" s="10"/>
+      <c r="Q10" s="10"/>
+      <c r="R10" s="10" t="s">
+        <v>39</v>
+      </c>
       <c r="S10" s="10"/>
       <c r="T10" s="10"/>
-    </row>
-    <row r="11" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="U10" s="10"/>
+      <c r="V10" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B11" s="5">
         <v>9</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>75</v>
+        <v>8</v>
       </c>
       <c r="D11" s="6">
-        <v>200139040</v>
+        <v>200137313</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>83</v>
+        <v>34</v>
       </c>
       <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
+      <c r="G11" s="10" t="s">
+        <v>39</v>
+      </c>
       <c r="H11" s="10"/>
       <c r="I11" s="10"/>
       <c r="J11" s="10"/>
@@ -1221,25 +1305,29 @@
       <c r="N11" s="10"/>
       <c r="O11" s="10"/>
       <c r="P11" s="10"/>
-      <c r="Q11" s="10"/>
+      <c r="Q11" s="10" t="s">
+        <v>39</v>
+      </c>
       <c r="R11" s="10"/>
       <c r="S11" s="10"/>
-      <c r="T11" s="10" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="12" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="T11" s="10"/>
+      <c r="U11" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="V11" s="10"/>
+    </row>
+    <row r="12" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B12" s="5">
         <v>10</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D12" s="6">
-        <v>200122995</v>
+        <v>200139040</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F12" s="10"/>
       <c r="G12" s="10"/>
@@ -1258,30 +1346,28 @@
       <c r="T12" s="10" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="13" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="U12" s="10"/>
+      <c r="V12" s="10"/>
+    </row>
+    <row r="13" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B13" s="5">
         <v>11</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>9</v>
+        <v>89</v>
       </c>
       <c r="D13" s="6">
-        <v>200137471</v>
+        <v>200135408</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>35</v>
+        <v>93</v>
       </c>
       <c r="F13" s="10"/>
       <c r="G13" s="10"/>
       <c r="H13" s="10"/>
       <c r="I13" s="10"/>
-      <c r="J13" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="K13" s="10" t="s">
-        <v>39</v>
-      </c>
+      <c r="J13" s="10"/>
+      <c r="K13" s="10"/>
       <c r="L13" s="10"/>
       <c r="M13" s="10"/>
       <c r="N13" s="10"/>
@@ -1289,23 +1375,25 @@
       <c r="P13" s="10"/>
       <c r="Q13" s="10"/>
       <c r="R13" s="10"/>
-      <c r="S13" s="10" t="s">
-        <v>39</v>
-      </c>
+      <c r="S13" s="10"/>
       <c r="T13" s="10"/>
-    </row>
-    <row r="14" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="U13" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="V13" s="10"/>
+    </row>
+    <row r="14" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B14" s="5">
         <v>12</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>10</v>
+        <v>79</v>
       </c>
       <c r="D14" s="6">
-        <v>200136596</v>
-      </c>
-      <c r="E14" s="8" t="s">
-        <v>36</v>
+        <v>200122995</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>84</v>
       </c>
       <c r="F14" s="10"/>
       <c r="G14" s="10"/>
@@ -1317,30 +1405,28 @@
       <c r="M14" s="10"/>
       <c r="N14" s="10"/>
       <c r="O14" s="10"/>
-      <c r="P14" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q14" s="10" t="s">
-        <v>39</v>
-      </c>
+      <c r="P14" s="10"/>
+      <c r="Q14" s="10"/>
       <c r="R14" s="10"/>
       <c r="S14" s="10"/>
       <c r="T14" s="10" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="15" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="U14" s="10"/>
+      <c r="V14" s="10"/>
+    </row>
+    <row r="15" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B15" s="5">
         <v>13</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D15" s="7">
-        <v>200137284</v>
+        <v>98</v>
+      </c>
+      <c r="D15" s="6">
+        <v>200134680</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>37</v>
+        <v>100</v>
       </c>
       <c r="F15" s="10"/>
       <c r="G15" s="10"/>
@@ -1353,89 +1439,105 @@
       <c r="N15" s="10"/>
       <c r="O15" s="10"/>
       <c r="P15" s="10"/>
-      <c r="Q15" s="10" t="s">
-        <v>39</v>
-      </c>
+      <c r="Q15" s="10"/>
       <c r="R15" s="10"/>
       <c r="S15" s="10"/>
-      <c r="T15" s="10" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="16" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="T15" s="10"/>
+      <c r="U15" s="10"/>
+      <c r="V15" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B16" s="5">
         <v>14</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D16" s="7">
-        <v>200135338</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>20</v>
+        <v>9</v>
+      </c>
+      <c r="D16" s="6">
+        <v>200137471</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>35</v>
       </c>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
       <c r="H16" s="10"/>
       <c r="I16" s="10"/>
-      <c r="J16" s="10"/>
-      <c r="K16" s="10"/>
+      <c r="J16" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="K16" s="10" t="s">
+        <v>39</v>
+      </c>
       <c r="L16" s="10"/>
       <c r="M16" s="10"/>
       <c r="N16" s="10"/>
       <c r="O16" s="10"/>
-      <c r="P16" s="10" t="s">
-        <v>39</v>
-      </c>
+      <c r="P16" s="10"/>
       <c r="Q16" s="10"/>
       <c r="R16" s="10"/>
-      <c r="S16" s="10"/>
+      <c r="S16" s="10" t="s">
+        <v>39</v>
+      </c>
       <c r="T16" s="10"/>
-    </row>
-    <row r="17" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="U16" s="10"/>
+      <c r="V16" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B17" s="5">
         <v>15</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D17" s="6">
-        <v>200048588</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>21</v>
+        <v>200136596</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>36</v>
       </c>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
       <c r="H17" s="10"/>
       <c r="I17" s="10"/>
       <c r="J17" s="10"/>
-      <c r="K17" s="10" t="s">
-        <v>39</v>
-      </c>
+      <c r="K17" s="10"/>
       <c r="L17" s="10"/>
       <c r="M17" s="10"/>
       <c r="N17" s="10"/>
       <c r="O17" s="10"/>
-      <c r="P17" s="10"/>
-      <c r="Q17" s="10"/>
+      <c r="P17" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q17" s="10" t="s">
+        <v>39</v>
+      </c>
       <c r="R17" s="10"/>
       <c r="S17" s="10"/>
-      <c r="T17" s="10"/>
-    </row>
-    <row r="18" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="T17" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="U17" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="V17" s="10"/>
+    </row>
+    <row r="18" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B18" s="5">
         <v>16</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D18" s="7">
-        <v>200082252</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>22</v>
+        <v>200137284</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>37</v>
       </c>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
@@ -1447,90 +1549,104 @@
       <c r="M18" s="10"/>
       <c r="N18" s="10"/>
       <c r="O18" s="10"/>
-      <c r="P18" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q18" s="10"/>
+      <c r="P18" s="10"/>
+      <c r="Q18" s="10" t="s">
+        <v>39</v>
+      </c>
       <c r="R18" s="10"/>
       <c r="S18" s="10"/>
-      <c r="T18" s="10"/>
-    </row>
-    <row r="19" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="T18" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="U18" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="V18" s="10"/>
+    </row>
+    <row r="19" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B19" s="5">
         <v>17</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D19" s="7">
-        <v>200136002</v>
+        <v>200135338</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F19" s="10"/>
       <c r="G19" s="10"/>
       <c r="H19" s="10"/>
       <c r="I19" s="10"/>
       <c r="J19" s="10"/>
-      <c r="K19" s="10" t="s">
-        <v>39</v>
-      </c>
+      <c r="K19" s="10"/>
       <c r="L19" s="10"/>
       <c r="M19" s="10"/>
       <c r="N19" s="10"/>
       <c r="O19" s="10"/>
-      <c r="P19" s="10"/>
+      <c r="P19" s="10" t="s">
+        <v>39</v>
+      </c>
       <c r="Q19" s="10"/>
       <c r="R19" s="10"/>
       <c r="S19" s="10"/>
-      <c r="T19" s="10" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="20" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="T19" s="10"/>
+      <c r="U19" s="10"/>
+      <c r="V19" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B20" s="5">
         <v>18</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D20" s="7">
-        <v>200135574</v>
+        <v>13</v>
+      </c>
+      <c r="D20" s="6">
+        <v>200048588</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F20" s="10"/>
       <c r="G20" s="10"/>
       <c r="H20" s="10"/>
       <c r="I20" s="10"/>
       <c r="J20" s="10"/>
-      <c r="K20" s="10"/>
+      <c r="K20" s="10" t="s">
+        <v>39</v>
+      </c>
       <c r="L20" s="10"/>
       <c r="M20" s="10"/>
       <c r="N20" s="10"/>
       <c r="O20" s="10"/>
-      <c r="P20" s="10" t="s">
-        <v>39</v>
-      </c>
+      <c r="P20" s="10"/>
       <c r="Q20" s="10"/>
       <c r="R20" s="10"/>
       <c r="S20" s="10"/>
       <c r="T20" s="10"/>
-    </row>
-    <row r="21" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="U20" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="V20" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B21" s="5">
         <v>19</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>77</v>
+        <v>14</v>
       </c>
       <c r="D21" s="7">
-        <v>200108882</v>
+        <v>200082252</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>85</v>
+        <v>22</v>
       </c>
       <c r="F21" s="10"/>
       <c r="G21" s="10"/>
@@ -1542,26 +1658,28 @@
       <c r="M21" s="10"/>
       <c r="N21" s="10"/>
       <c r="O21" s="10"/>
-      <c r="P21" s="10"/>
+      <c r="P21" s="10" t="s">
+        <v>39</v>
+      </c>
       <c r="Q21" s="10"/>
       <c r="R21" s="10"/>
       <c r="S21" s="10"/>
-      <c r="T21" s="10" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="22" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="T21" s="10"/>
+      <c r="U21" s="10"/>
+      <c r="V21" s="10"/>
+    </row>
+    <row r="22" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B22" s="5">
         <v>20</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D22" s="6">
-        <v>200109296</v>
+        <v>97</v>
+      </c>
+      <c r="D22" s="7">
+        <v>200108361</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>25</v>
+        <v>101</v>
       </c>
       <c r="F22" s="10"/>
       <c r="G22" s="10"/>
@@ -1571,38 +1689,36 @@
       <c r="K22" s="10"/>
       <c r="L22" s="10"/>
       <c r="M22" s="10"/>
-      <c r="N22" s="10" t="s">
-        <v>39</v>
-      </c>
+      <c r="N22" s="10"/>
       <c r="O22" s="10"/>
       <c r="P22" s="10"/>
       <c r="Q22" s="10"/>
       <c r="R22" s="10"/>
       <c r="S22" s="10"/>
-      <c r="T22" s="10" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="23" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="T22" s="10"/>
+      <c r="U22" s="10"/>
+      <c r="V22" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B23" s="5">
         <v>21</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D23" s="7">
-        <v>200134170</v>
+        <v>200136002</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F23" s="10"/>
       <c r="G23" s="10"/>
       <c r="H23" s="10"/>
       <c r="I23" s="10"/>
-      <c r="J23" s="10" t="s">
-        <v>39</v>
-      </c>
+      <c r="J23" s="10"/>
       <c r="K23" s="10" t="s">
         <v>39</v>
       </c>
@@ -1611,65 +1727,69 @@
       <c r="N23" s="10"/>
       <c r="O23" s="10"/>
       <c r="P23" s="10"/>
-      <c r="Q23" s="10" t="s">
-        <v>39</v>
-      </c>
+      <c r="Q23" s="10"/>
       <c r="R23" s="10"/>
       <c r="S23" s="10"/>
-      <c r="T23" s="10"/>
-    </row>
-    <row r="24" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="T23" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="U23" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="V23" s="10"/>
+    </row>
+    <row r="24" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B24" s="5">
         <v>22</v>
       </c>
-      <c r="C24" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="D24" s="6">
-        <v>200107036</v>
+      <c r="C24" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D24" s="7">
+        <v>200135574</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F24" s="10"/>
       <c r="G24" s="10"/>
       <c r="H24" s="10"/>
-      <c r="I24" s="10" t="s">
-        <v>39</v>
-      </c>
+      <c r="I24" s="10"/>
       <c r="J24" s="10"/>
       <c r="K24" s="10"/>
       <c r="L24" s="10"/>
       <c r="M24" s="10"/>
       <c r="N24" s="10"/>
       <c r="O24" s="10"/>
-      <c r="P24" s="10"/>
+      <c r="P24" s="10" t="s">
+        <v>39</v>
+      </c>
       <c r="Q24" s="10"/>
       <c r="R24" s="10"/>
       <c r="S24" s="10"/>
-      <c r="T24" s="10" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="25" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="T24" s="10"/>
+      <c r="U24" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="V24" s="10"/>
+    </row>
+    <row r="25" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B25" s="5">
         <v>23</v>
       </c>
-      <c r="C25" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="D25" s="6">
-        <v>200107506</v>
+      <c r="C25" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="D25" s="7">
+        <v>200108882</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F25" s="10"/>
       <c r="G25" s="10"/>
       <c r="H25" s="10"/>
-      <c r="I25" s="10" t="s">
-        <v>39</v>
-      </c>
+      <c r="I25" s="10"/>
       <c r="J25" s="10"/>
       <c r="K25" s="10"/>
       <c r="L25" s="10"/>
@@ -1683,6 +1803,189 @@
       <c r="T25" s="10" t="s">
         <v>39</v>
       </c>
+      <c r="U25" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="V25" s="10"/>
+    </row>
+    <row r="26" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="B26" s="5">
+        <v>24</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D26" s="6">
+        <v>200109296</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F26" s="10"/>
+      <c r="G26" s="10"/>
+      <c r="H26" s="10"/>
+      <c r="I26" s="10"/>
+      <c r="J26" s="10"/>
+      <c r="K26" s="10"/>
+      <c r="L26" s="10"/>
+      <c r="M26" s="10"/>
+      <c r="N26" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="O26" s="10"/>
+      <c r="P26" s="10"/>
+      <c r="Q26" s="10"/>
+      <c r="R26" s="10"/>
+      <c r="S26" s="10"/>
+      <c r="T26" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="U26" s="10"/>
+      <c r="V26" s="10"/>
+    </row>
+    <row r="27" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="B27" s="5">
+        <v>25</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D27" s="7">
+        <v>200134170</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F27" s="10"/>
+      <c r="G27" s="10"/>
+      <c r="H27" s="10"/>
+      <c r="I27" s="10"/>
+      <c r="J27" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="K27" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="L27" s="10"/>
+      <c r="M27" s="10"/>
+      <c r="N27" s="10"/>
+      <c r="O27" s="10"/>
+      <c r="P27" s="10"/>
+      <c r="Q27" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="R27" s="10"/>
+      <c r="S27" s="10"/>
+      <c r="T27" s="10"/>
+      <c r="U27" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="V27" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="28" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="B28" s="5">
+        <v>26</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="D28" s="7">
+        <v>200134299</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="F28" s="10"/>
+      <c r="G28" s="10"/>
+      <c r="H28" s="10"/>
+      <c r="I28" s="10"/>
+      <c r="J28" s="10"/>
+      <c r="K28" s="10"/>
+      <c r="L28" s="10"/>
+      <c r="M28" s="10"/>
+      <c r="N28" s="10"/>
+      <c r="O28" s="10"/>
+      <c r="P28" s="10"/>
+      <c r="Q28" s="10"/>
+      <c r="R28" s="10"/>
+      <c r="S28" s="10"/>
+      <c r="T28" s="10"/>
+      <c r="U28" s="10"/>
+      <c r="V28" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="29" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="B29" s="5">
+        <v>27</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D29" s="6">
+        <v>200107036</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F29" s="10"/>
+      <c r="G29" s="10"/>
+      <c r="H29" s="10"/>
+      <c r="I29" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="J29" s="10"/>
+      <c r="K29" s="10"/>
+      <c r="L29" s="10"/>
+      <c r="M29" s="10"/>
+      <c r="N29" s="10"/>
+      <c r="O29" s="10"/>
+      <c r="P29" s="10"/>
+      <c r="Q29" s="10"/>
+      <c r="R29" s="10"/>
+      <c r="S29" s="10"/>
+      <c r="T29" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="U29" s="10"/>
+      <c r="V29" s="10"/>
+    </row>
+    <row r="30" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="B30" s="5">
+        <v>28</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="D30" s="6">
+        <v>200107506</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="F30" s="10"/>
+      <c r="G30" s="10"/>
+      <c r="H30" s="10"/>
+      <c r="I30" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="J30" s="10"/>
+      <c r="K30" s="10"/>
+      <c r="L30" s="10"/>
+      <c r="M30" s="10"/>
+      <c r="N30" s="10"/>
+      <c r="O30" s="10"/>
+      <c r="P30" s="10"/>
+      <c r="Q30" s="10"/>
+      <c r="R30" s="10"/>
+      <c r="S30" s="10"/>
+      <c r="T30" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="U30" s="10"/>
+      <c r="V30" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1692,10 +1995,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53390297-B1EB-4F05-BF18-BF0D31A69F5E}">
-  <dimension ref="B2:E17"/>
+  <dimension ref="B2:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1922,7 +2225,36 @@
         <v>87</v>
       </c>
     </row>
+    <row r="18" spans="2:5" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="B18" s="15">
+        <v>44282</v>
+      </c>
+      <c r="C18" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="D18" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="E18" s="19" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" ht="55.2" x14ac:dyDescent="0.3">
+      <c r="B19" s="15">
+        <v>44295</v>
+      </c>
+      <c r="C19" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="D19" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="E19" s="20" t="s">
+        <v>94</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="14" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="E4" r:id="rId1" xr:uid="{C15FC39B-8594-40E1-AE9B-6B3764FCA922}"/>
     <hyperlink ref="E6" r:id="rId2" xr:uid="{13CC4F08-94C1-42F9-88CD-E695A77E9D8C}"/>
@@ -1931,8 +2263,9 @@
     <hyperlink ref="E14" r:id="rId5" xr:uid="{38265528-8FD6-4712-9CE9-5D3C234C19EB}"/>
     <hyperlink ref="E8" r:id="rId6" xr:uid="{503BBAA4-5A6A-4978-A1DC-56DF48E93E0A}"/>
     <hyperlink ref="E17" r:id="rId7" xr:uid="{65123D90-E02A-4775-9E7C-4354D603709B}"/>
+    <hyperlink ref="E19" r:id="rId8" xr:uid="{BD699360-E531-49E4-8141-D5A0F3FF9101}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId8"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="1200" r:id="rId9"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Funciones Recursivas 2D pt. 1
</commit_message>
<xml_diff>
--- a/Asistencia/AsistenciaMonitoriaED_2021_1_EnriqueNiebles.xlsx
+++ b/Asistencia/AsistenciaMonitoriaED_2021_1_EnriqueNiebles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Enrique Niebles\Documents\Universidad del Norte\Ingeniería Electrónica - Sistemas y Computación\7. Séptimo Semestre\Monitoria Estructuras Discretas\Material\Asistencia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17E0726A-C63D-4EE7-81D1-C823EF1F9987}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE3C4F3D-2E58-4C83-B669-D5C0E6301E14}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1068" yWindow="-108" windowWidth="22080" windowHeight="13176" xr2:uid="{9F616065-CB98-49F1-BECD-2AD80A2EEE2C}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="111">
   <si>
     <t>Estudiante</t>
   </si>
@@ -359,6 +359,15 @@
   </si>
   <si>
     <t>https://drive.google.com/file/d/1CClrMMmwj_kR_tJCbd6eFfZiRr5Qf0I7/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>Funciones recursivas 2D pt. 1</t>
+  </si>
+  <si>
+    <t>Se explicó cómo trabajar con funciones recursivas en 2D. Se aclararon conceptos, se porgramó en Python y se recomendó realizar nuevamente los diseños en MATLAB. Así mismo, se dejó un ejercicio para que practicaran.</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1mxm_8XblzECmnZt89HTQRVeJ58YJFx52/view?usp=sharing</t>
   </si>
 </sst>
 </file>
@@ -919,8 +928,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23B5D081-BD4A-44D4-A2DC-90E7E1D86DF5}">
   <dimension ref="B2:BB30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Y12" sqref="Y12"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AA16" sqref="AA16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -931,10 +940,11 @@
     <col min="4" max="4" width="14.09765625" style="1" customWidth="1"/>
     <col min="5" max="5" width="19.19921875" style="1" customWidth="1"/>
     <col min="6" max="23" width="11.19921875" style="1" hidden="1" customWidth="1"/>
-    <col min="24" max="54" width="11.19921875" style="1"/>
+    <col min="24" max="24" width="0" style="1" hidden="1" customWidth="1"/>
+    <col min="25" max="54" width="11.19921875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:24" ht="18" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:25" ht="18" x14ac:dyDescent="0.3">
       <c r="B2" s="3"/>
       <c r="C2" s="4" t="s">
         <v>0</v>
@@ -1002,8 +1012,11 @@
       <c r="X2" s="9">
         <v>44309</v>
       </c>
-    </row>
-    <row r="3" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="Y2" s="9">
+        <v>44310</v>
+      </c>
+    </row>
+    <row r="3" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B3" s="5">
         <v>1</v>
       </c>
@@ -1051,8 +1064,11 @@
       <c r="X3" s="10" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="4" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="Y3" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B4" s="5">
         <v>2</v>
       </c>
@@ -1086,8 +1102,9 @@
       <c r="V4" s="10"/>
       <c r="W4" s="10"/>
       <c r="X4" s="10"/>
-    </row>
-    <row r="5" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="Y4" s="10"/>
+    </row>
+    <row r="5" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B5" s="5">
         <v>3</v>
       </c>
@@ -1121,8 +1138,9 @@
       <c r="V5" s="10"/>
       <c r="W5" s="10"/>
       <c r="X5" s="10"/>
-    </row>
-    <row r="6" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="Y5" s="10"/>
+    </row>
+    <row r="6" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B6" s="5">
         <v>4</v>
       </c>
@@ -1156,8 +1174,9 @@
       <c r="V6" s="10"/>
       <c r="W6" s="10"/>
       <c r="X6" s="10"/>
-    </row>
-    <row r="7" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="Y6" s="10"/>
+    </row>
+    <row r="7" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B7" s="5">
         <v>5</v>
       </c>
@@ -1199,8 +1218,9 @@
         <v>39</v>
       </c>
       <c r="X7" s="10"/>
-    </row>
-    <row r="8" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="Y7" s="10"/>
+    </row>
+    <row r="8" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B8" s="5">
         <v>6</v>
       </c>
@@ -1238,8 +1258,9 @@
       <c r="V8" s="10"/>
       <c r="W8" s="10"/>
       <c r="X8" s="10"/>
-    </row>
-    <row r="9" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="Y8" s="10"/>
+    </row>
+    <row r="9" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B9" s="5">
         <v>7</v>
       </c>
@@ -1283,8 +1304,9 @@
       <c r="X9" s="10" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="10" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="Y9" s="10"/>
+    </row>
+    <row r="10" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B10" s="5">
         <v>8</v>
       </c>
@@ -1324,8 +1346,9 @@
         <v>39</v>
       </c>
       <c r="X10" s="10"/>
-    </row>
-    <row r="11" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="Y10" s="10"/>
+    </row>
+    <row r="11" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B11" s="5">
         <v>9</v>
       </c>
@@ -1365,8 +1388,11 @@
       <c r="X11" s="10" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="12" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="Y11" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B12" s="5">
         <v>10</v>
       </c>
@@ -1400,8 +1426,9 @@
       <c r="V12" s="10"/>
       <c r="W12" s="10"/>
       <c r="X12" s="10"/>
-    </row>
-    <row r="13" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="Y12" s="10"/>
+    </row>
+    <row r="13" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B13" s="5">
         <v>11</v>
       </c>
@@ -1435,8 +1462,9 @@
       <c r="V13" s="10"/>
       <c r="W13" s="10"/>
       <c r="X13" s="10"/>
-    </row>
-    <row r="14" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="Y13" s="10"/>
+    </row>
+    <row r="14" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B14" s="5">
         <v>12</v>
       </c>
@@ -1470,8 +1498,9 @@
       <c r="V14" s="10"/>
       <c r="W14" s="10"/>
       <c r="X14" s="10"/>
-    </row>
-    <row r="15" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="Y14" s="10"/>
+    </row>
+    <row r="15" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B15" s="5">
         <v>13</v>
       </c>
@@ -1505,8 +1534,9 @@
       </c>
       <c r="W15" s="10"/>
       <c r="X15" s="10"/>
-    </row>
-    <row r="16" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="Y15" s="10"/>
+    </row>
+    <row r="16" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B16" s="5">
         <v>14</v>
       </c>
@@ -1548,8 +1578,9 @@
       <c r="X16" s="10" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="17" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="Y16" s="10"/>
+    </row>
+    <row r="17" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B17" s="5">
         <v>15</v>
       </c>
@@ -1589,8 +1620,11 @@
       <c r="V17" s="10"/>
       <c r="W17" s="10"/>
       <c r="X17" s="10"/>
-    </row>
-    <row r="18" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="Y17" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B18" s="5">
         <v>16</v>
       </c>
@@ -1628,8 +1662,9 @@
       <c r="V18" s="10"/>
       <c r="W18" s="10"/>
       <c r="X18" s="10"/>
-    </row>
-    <row r="19" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="Y18" s="10"/>
+    </row>
+    <row r="19" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B19" s="5">
         <v>17</v>
       </c>
@@ -1665,8 +1700,9 @@
       </c>
       <c r="W19" s="10"/>
       <c r="X19" s="10"/>
-    </row>
-    <row r="20" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="Y19" s="10"/>
+    </row>
+    <row r="20" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B20" s="5">
         <v>18</v>
       </c>
@@ -1706,8 +1742,9 @@
       <c r="X20" s="10" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="21" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="Y20" s="10"/>
+    </row>
+    <row r="21" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B21" s="5">
         <v>19</v>
       </c>
@@ -1741,8 +1778,9 @@
       <c r="V21" s="10"/>
       <c r="W21" s="10"/>
       <c r="X21" s="10"/>
-    </row>
-    <row r="22" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="Y21" s="10"/>
+    </row>
+    <row r="22" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B22" s="5">
         <v>20</v>
       </c>
@@ -1776,8 +1814,9 @@
       </c>
       <c r="W22" s="10"/>
       <c r="X22" s="10"/>
-    </row>
-    <row r="23" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="Y22" s="10"/>
+    </row>
+    <row r="23" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B23" s="5">
         <v>21</v>
       </c>
@@ -1815,8 +1854,9 @@
       <c r="V23" s="10"/>
       <c r="W23" s="10"/>
       <c r="X23" s="10"/>
-    </row>
-    <row r="24" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="Y23" s="10"/>
+    </row>
+    <row r="24" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B24" s="5">
         <v>22</v>
       </c>
@@ -1852,8 +1892,9 @@
       <c r="V24" s="10"/>
       <c r="W24" s="10"/>
       <c r="X24" s="10"/>
-    </row>
-    <row r="25" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="Y24" s="10"/>
+    </row>
+    <row r="25" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B25" s="5">
         <v>23</v>
       </c>
@@ -1889,8 +1930,9 @@
       <c r="V25" s="10"/>
       <c r="W25" s="10"/>
       <c r="X25" s="10"/>
-    </row>
-    <row r="26" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="Y25" s="10"/>
+    </row>
+    <row r="26" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B26" s="5">
         <v>24</v>
       </c>
@@ -1926,8 +1968,9 @@
       <c r="V26" s="10"/>
       <c r="W26" s="10"/>
       <c r="X26" s="10"/>
-    </row>
-    <row r="27" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="Y26" s="10"/>
+    </row>
+    <row r="27" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B27" s="5">
         <v>25</v>
       </c>
@@ -1969,8 +2012,9 @@
       </c>
       <c r="W27" s="10"/>
       <c r="X27" s="10"/>
-    </row>
-    <row r="28" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="Y27" s="10"/>
+    </row>
+    <row r="28" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B28" s="5">
         <v>26</v>
       </c>
@@ -2004,8 +2048,9 @@
       </c>
       <c r="W28" s="10"/>
       <c r="X28" s="10"/>
-    </row>
-    <row r="29" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="Y28" s="10"/>
+    </row>
+    <row r="29" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B29" s="5">
         <v>27</v>
       </c>
@@ -2041,8 +2086,9 @@
       <c r="V29" s="10"/>
       <c r="W29" s="10"/>
       <c r="X29" s="10"/>
-    </row>
-    <row r="30" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="Y29" s="10"/>
+    </row>
+    <row r="30" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B30" s="5">
         <v>28</v>
       </c>
@@ -2078,6 +2124,7 @@
       <c r="V30" s="10"/>
       <c r="W30" s="10"/>
       <c r="X30" s="10"/>
+      <c r="Y30" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2087,10 +2134,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53390297-B1EB-4F05-BF18-BF0D31A69F5E}">
-  <dimension ref="B2:E21"/>
+  <dimension ref="B2:E22"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2371,6 +2418,20 @@
       </c>
       <c r="E21" s="20" t="s">
         <v>107</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" ht="55.2" x14ac:dyDescent="0.3">
+      <c r="B22" s="15">
+        <v>44316</v>
+      </c>
+      <c r="C22" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="D22" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="E22" s="20" t="s">
+        <v>110</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Asistencia y bot actualizada.
</commit_message>
<xml_diff>
--- a/Asistencia/AsistenciaMonitoriaED_2021_1_EnriqueNiebles.xlsx
+++ b/Asistencia/AsistenciaMonitoriaED_2021_1_EnriqueNiebles.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Enrique Niebles\Documents\Universidad del Norte\Ingeniería Electrónica - Sistemas y Computación\7. Séptimo Semestre\Monitoria Estructuras Discretas\Material\Asistencia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55416E57-F399-4519-981D-4AC4B8756427}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E031723-64D0-44A3-89DD-67690DC677B9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1068" yWindow="-108" windowWidth="22080" windowHeight="13176" activeTab="1" xr2:uid="{9F616065-CB98-49F1-BECD-2AD80A2EEE2C}"/>
+    <workbookView xWindow="1068" yWindow="-108" windowWidth="22080" windowHeight="13176" xr2:uid="{9F616065-CB98-49F1-BECD-2AD80A2EEE2C}"/>
   </bookViews>
   <sheets>
     <sheet name="Asistencia" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="134">
   <si>
     <t>Estudiante</t>
   </si>
@@ -389,13 +389,61 @@
   </si>
   <si>
     <t>Se explicó cómo crear en bots de Telegram. También, se enfocó en el envío de documentos, imágenes, y manejo de texto recibido por un usuario.</t>
+  </si>
+  <si>
+    <t>Solución dudas bot</t>
+  </si>
+  <si>
+    <t>Solución dudas bot + nuevas funciones/librerías</t>
+  </si>
+  <si>
+    <t>Solución dudas y errores de Python.</t>
+  </si>
+  <si>
+    <t>Se ayudó a un grupo a resolver los errores de ejecución de su programa y se brindó una guía para resolver el primer punto del bot.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se continuaron resolviendo dudas relacionadas con el desarrollo del bot y las posibles librerías que podían implementar en sus soluciones, así como funciones que podían serles útiles, tanto para graficar como para simplificar ecuaciones. </t>
+  </si>
+  <si>
+    <t>Sebastian Manuel Guzman Hernandez</t>
+  </si>
+  <si>
+    <t>guzmanms</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/17Mt9zQxOuy7ILGTVu0urTp62OWK6rQ8-/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>Se habilitó un espacio para que resolver dudas del proyecto computacional y del bot. Así mismo, se hizo un repaso para que pudiesen familiarizarse más con lo realizado en la monitoria anterior. También, se presentaron algunas librerías que pueden implementar para graficar los grafos y evaluar funciones.</t>
+  </si>
+  <si>
+    <t>Freddy David Guete Maldonado</t>
+  </si>
+  <si>
+    <t>fguete</t>
+  </si>
+  <si>
+    <t>Total Asistencias</t>
+  </si>
+  <si>
+    <t>Sin asistencias</t>
+  </si>
+  <si>
+    <t>Recuento</t>
+  </si>
+  <si>
+    <t>Luis Felipe Evilla Rodriguez</t>
+  </si>
+  <si>
+    <t>lfevilla</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -506,13 +554,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="4">
@@ -569,7 +631,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -631,6 +693,18 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -947,25 +1021,46 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23B5D081-BD4A-44D4-A2DC-90E7E1D86DF5}">
-  <dimension ref="B2:BB32"/>
+  <dimension ref="B1:BB36"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="P22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AC39" sqref="AC39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="2" customWidth="1"/>
     <col min="2" max="2" width="4.09765625" customWidth="1"/>
-    <col min="3" max="3" width="38.19921875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="14.09765625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="19.19921875" style="1" customWidth="1"/>
-    <col min="6" max="23" width="11.19921875" style="1" hidden="1" customWidth="1"/>
-    <col min="24" max="25" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="26" max="54" width="11.19921875" style="1"/>
+    <col min="3" max="3" width="35.19921875" style="2" customWidth="1"/>
+    <col min="4" max="5" width="14.09765625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.796875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="11.19921875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="13.796875" style="1" customWidth="1"/>
+    <col min="9" max="12" width="11.19921875" style="1" customWidth="1"/>
+    <col min="13" max="13" width="14.09765625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="11.19921875" style="1" customWidth="1"/>
+    <col min="15" max="15" width="13.796875" style="1" customWidth="1"/>
+    <col min="16" max="25" width="11.19921875" style="1" customWidth="1"/>
+    <col min="26" max="29" width="11.19921875" style="1"/>
+    <col min="30" max="30" width="13.69921875" style="1" customWidth="1"/>
+    <col min="31" max="54" width="11.19921875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:26" ht="18" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:30" x14ac:dyDescent="0.3">
+      <c r="F1" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="H1" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="M1" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="O1" s="22" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="2" spans="2:30" ht="36" x14ac:dyDescent="0.3">
       <c r="B2" s="3"/>
       <c r="C2" s="4" t="s">
         <v>0</v>
@@ -973,7 +1068,7 @@
       <c r="D2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="23" t="s">
         <v>38</v>
       </c>
       <c r="F2" s="11">
@@ -1039,8 +1134,20 @@
       <c r="Z2" s="9">
         <v>44323</v>
       </c>
-    </row>
-    <row r="3" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="AA2" s="9">
+        <v>44330</v>
+      </c>
+      <c r="AB2" s="9">
+        <v>44337</v>
+      </c>
+      <c r="AC2" s="9">
+        <v>44338</v>
+      </c>
+      <c r="AD2" s="9" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="3" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B3" s="5">
         <v>1</v>
       </c>
@@ -1094,8 +1201,17 @@
       <c r="Z3" s="10" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="4" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="AA3" s="10"/>
+      <c r="AB3" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC3" s="10"/>
+      <c r="AD3" s="10">
+        <f t="shared" ref="AD3:AD13" si="0">COUNTIF(F3:AC3,"X")</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B4" s="5">
         <v>2</v>
       </c>
@@ -1131,8 +1247,15 @@
       <c r="X4" s="10"/>
       <c r="Y4" s="10"/>
       <c r="Z4" s="10"/>
-    </row>
-    <row r="5" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="AA4" s="10"/>
+      <c r="AB4" s="10"/>
+      <c r="AC4" s="10"/>
+      <c r="AD4" s="10">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B5" s="5">
         <v>3</v>
       </c>
@@ -1168,8 +1291,15 @@
       <c r="X5" s="10"/>
       <c r="Y5" s="10"/>
       <c r="Z5" s="10"/>
-    </row>
-    <row r="6" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="AA5" s="10"/>
+      <c r="AB5" s="10"/>
+      <c r="AC5" s="10"/>
+      <c r="AD5" s="10">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B6" s="5">
         <v>4</v>
       </c>
@@ -1205,8 +1335,15 @@
       <c r="X6" s="10"/>
       <c r="Y6" s="10"/>
       <c r="Z6" s="10"/>
-    </row>
-    <row r="7" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="AA6" s="10"/>
+      <c r="AB6" s="10"/>
+      <c r="AC6" s="10"/>
+      <c r="AD6" s="10">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B7" s="5">
         <v>5</v>
       </c>
@@ -1250,8 +1387,15 @@
       <c r="X7" s="10"/>
       <c r="Y7" s="10"/>
       <c r="Z7" s="10"/>
-    </row>
-    <row r="8" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="AA7" s="10"/>
+      <c r="AB7" s="10"/>
+      <c r="AC7" s="10"/>
+      <c r="AD7" s="10">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B8" s="5">
         <v>6</v>
       </c>
@@ -1291,8 +1435,15 @@
       <c r="X8" s="10"/>
       <c r="Y8" s="10"/>
       <c r="Z8" s="10"/>
-    </row>
-    <row r="9" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="AA8" s="10"/>
+      <c r="AB8" s="10"/>
+      <c r="AC8" s="10"/>
+      <c r="AD8" s="10">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B9" s="5">
         <v>7</v>
       </c>
@@ -1328,8 +1479,15 @@
       <c r="Z9" s="10" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="10" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="AA9" s="10"/>
+      <c r="AB9" s="10"/>
+      <c r="AC9" s="10"/>
+      <c r="AD9" s="10">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B10" s="5">
         <v>8</v>
       </c>
@@ -1377,8 +1535,17 @@
       <c r="Z10" s="10" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="11" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="AA10" s="10"/>
+      <c r="AB10" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC10" s="10"/>
+      <c r="AD10" s="10">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B11" s="5">
         <v>9</v>
       </c>
@@ -1420,8 +1587,17 @@
       <c r="X11" s="10"/>
       <c r="Y11" s="10"/>
       <c r="Z11" s="10"/>
-    </row>
-    <row r="12" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="AA11" s="10"/>
+      <c r="AB11" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC11" s="10"/>
+      <c r="AD11" s="10">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B12" s="5">
         <v>10</v>
       </c>
@@ -1467,8 +1643,17 @@
       <c r="Z12" s="10" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="13" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="AA12" s="10"/>
+      <c r="AB12" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC12" s="10"/>
+      <c r="AD12" s="10">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B13" s="5">
         <v>11</v>
       </c>
@@ -1504,19 +1689,26 @@
       <c r="X13" s="10"/>
       <c r="Y13" s="10"/>
       <c r="Z13" s="10"/>
-    </row>
-    <row r="14" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="AA13" s="10"/>
+      <c r="AB13" s="10"/>
+      <c r="AC13" s="10"/>
+      <c r="AD13" s="10">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B14" s="5">
         <v>12</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>89</v>
+        <v>127</v>
       </c>
       <c r="D14" s="6">
-        <v>200135408</v>
+        <v>200137150</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>93</v>
+        <v>128</v>
       </c>
       <c r="F14" s="10"/>
       <c r="G14" s="10"/>
@@ -1533,27 +1725,34 @@
       <c r="R14" s="10"/>
       <c r="S14" s="10"/>
       <c r="T14" s="10"/>
-      <c r="U14" s="10" t="s">
-        <v>39</v>
-      </c>
+      <c r="U14" s="10"/>
       <c r="V14" s="10"/>
       <c r="W14" s="10"/>
       <c r="X14" s="10"/>
       <c r="Y14" s="10"/>
       <c r="Z14" s="10"/>
-    </row>
-    <row r="15" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="AA14" s="10"/>
+      <c r="AB14" s="10"/>
+      <c r="AC14" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD14" s="10">
+        <f>COUNTIF(F14:AC14,"X")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B15" s="5">
         <v>13</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="D15" s="6">
-        <v>200122995</v>
+        <v>200135408</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="F15" s="10"/>
       <c r="G15" s="10"/>
@@ -1569,28 +1768,35 @@
       <c r="Q15" s="10"/>
       <c r="R15" s="10"/>
       <c r="S15" s="10"/>
-      <c r="T15" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="U15" s="10"/>
+      <c r="T15" s="10"/>
+      <c r="U15" s="10" t="s">
+        <v>39</v>
+      </c>
       <c r="V15" s="10"/>
       <c r="W15" s="10"/>
       <c r="X15" s="10"/>
       <c r="Y15" s="10"/>
       <c r="Z15" s="10"/>
-    </row>
-    <row r="16" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="AA15" s="10"/>
+      <c r="AB15" s="10"/>
+      <c r="AC15" s="10"/>
+      <c r="AD15" s="10">
+        <f t="shared" ref="AD15:AD35" si="1">COUNTIF(F15:AC15,"X")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B16" s="5">
         <v>14</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>98</v>
+        <v>79</v>
       </c>
       <c r="D16" s="6">
-        <v>200134680</v>
+        <v>200122995</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
@@ -1606,28 +1812,35 @@
       <c r="Q16" s="10"/>
       <c r="R16" s="10"/>
       <c r="S16" s="10"/>
-      <c r="T16" s="10"/>
+      <c r="T16" s="10" t="s">
+        <v>39</v>
+      </c>
       <c r="U16" s="10"/>
-      <c r="V16" s="10" t="s">
-        <v>39</v>
-      </c>
+      <c r="V16" s="10"/>
       <c r="W16" s="10"/>
       <c r="X16" s="10"/>
       <c r="Y16" s="10"/>
       <c r="Z16" s="10"/>
-    </row>
-    <row r="17" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="AA16" s="10"/>
+      <c r="AB16" s="10"/>
+      <c r="AC16" s="10"/>
+      <c r="AD16" s="10">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B17" s="5">
         <v>15</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
       <c r="D17" s="6">
-        <v>200123907</v>
+        <v>200134680</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
@@ -1645,37 +1858,40 @@
       <c r="S17" s="10"/>
       <c r="T17" s="10"/>
       <c r="U17" s="10"/>
-      <c r="V17" s="10"/>
+      <c r="V17" s="10" t="s">
+        <v>39</v>
+      </c>
       <c r="W17" s="10"/>
       <c r="X17" s="10"/>
       <c r="Y17" s="10"/>
-      <c r="Z17" s="10" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="18" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="Z17" s="10"/>
+      <c r="AA17" s="10"/>
+      <c r="AB17" s="10"/>
+      <c r="AC17" s="10"/>
+      <c r="AD17" s="10">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B18" s="5">
         <v>16</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>9</v>
+        <v>112</v>
       </c>
       <c r="D18" s="6">
-        <v>200137471</v>
+        <v>200123907</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>35</v>
+        <v>113</v>
       </c>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
       <c r="H18" s="10"/>
       <c r="I18" s="10"/>
-      <c r="J18" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="K18" s="10" t="s">
-        <v>39</v>
-      </c>
+      <c r="J18" s="10"/>
+      <c r="K18" s="10"/>
       <c r="L18" s="10"/>
       <c r="M18" s="10"/>
       <c r="N18" s="10"/>
@@ -1683,80 +1899,90 @@
       <c r="P18" s="10"/>
       <c r="Q18" s="10"/>
       <c r="R18" s="10"/>
-      <c r="S18" s="10" t="s">
-        <v>39</v>
-      </c>
+      <c r="S18" s="10"/>
       <c r="T18" s="10"/>
       <c r="U18" s="10"/>
-      <c r="V18" s="10" t="s">
-        <v>39</v>
-      </c>
+      <c r="V18" s="10"/>
       <c r="W18" s="10"/>
-      <c r="X18" s="10" t="s">
-        <v>39</v>
-      </c>
+      <c r="X18" s="10"/>
       <c r="Y18" s="10"/>
-      <c r="Z18" s="10"/>
-    </row>
-    <row r="19" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="Z18" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="AA18" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="AB18" s="10"/>
+      <c r="AC18" s="10"/>
+      <c r="AD18" s="10">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B19" s="5">
         <v>17</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D19" s="6">
-        <v>200136596</v>
-      </c>
-      <c r="E19" s="8" t="s">
-        <v>36</v>
+        <v>200137471</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>35</v>
       </c>
       <c r="F19" s="10"/>
       <c r="G19" s="10"/>
       <c r="H19" s="10"/>
       <c r="I19" s="10"/>
-      <c r="J19" s="10"/>
-      <c r="K19" s="10"/>
+      <c r="J19" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="K19" s="10" t="s">
+        <v>39</v>
+      </c>
       <c r="L19" s="10"/>
       <c r="M19" s="10"/>
       <c r="N19" s="10"/>
       <c r="O19" s="10"/>
-      <c r="P19" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q19" s="10" t="s">
-        <v>39</v>
-      </c>
+      <c r="P19" s="10"/>
+      <c r="Q19" s="10"/>
       <c r="R19" s="10"/>
-      <c r="S19" s="10"/>
-      <c r="T19" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="U19" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="V19" s="10"/>
+      <c r="S19" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="T19" s="10"/>
+      <c r="U19" s="10"/>
+      <c r="V19" s="10" t="s">
+        <v>39</v>
+      </c>
       <c r="W19" s="10"/>
-      <c r="X19" s="10"/>
-      <c r="Y19" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="Z19" s="10" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="20" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="X19" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y19" s="10"/>
+      <c r="Z19" s="10"/>
+      <c r="AA19" s="10"/>
+      <c r="AB19" s="10"/>
+      <c r="AC19" s="10"/>
+      <c r="AD19" s="10">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B20" s="5">
         <v>18</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D20" s="7">
-        <v>200137284</v>
-      </c>
-      <c r="E20" s="7" t="s">
-        <v>37</v>
+        <v>10</v>
+      </c>
+      <c r="D20" s="6">
+        <v>200136596</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>36</v>
       </c>
       <c r="F20" s="10"/>
       <c r="G20" s="10"/>
@@ -1768,7 +1994,9 @@
       <c r="M20" s="10"/>
       <c r="N20" s="10"/>
       <c r="O20" s="10"/>
-      <c r="P20" s="10"/>
+      <c r="P20" s="10" t="s">
+        <v>39</v>
+      </c>
       <c r="Q20" s="10" t="s">
         <v>39</v>
       </c>
@@ -1783,21 +2011,32 @@
       <c r="V20" s="10"/>
       <c r="W20" s="10"/>
       <c r="X20" s="10"/>
-      <c r="Y20" s="10"/>
-      <c r="Z20" s="10"/>
-    </row>
-    <row r="21" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="Y20" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z20" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="AA20" s="10"/>
+      <c r="AB20" s="10"/>
+      <c r="AC20" s="10"/>
+      <c r="AD20" s="10">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B21" s="5">
         <v>19</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D21" s="7">
-        <v>200135338</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>20</v>
+        <v>200137284</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>37</v>
       </c>
       <c r="F21" s="10"/>
       <c r="G21" s="10"/>
@@ -1809,77 +2048,89 @@
       <c r="M21" s="10"/>
       <c r="N21" s="10"/>
       <c r="O21" s="10"/>
-      <c r="P21" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q21" s="10"/>
+      <c r="P21" s="10"/>
+      <c r="Q21" s="10" t="s">
+        <v>39</v>
+      </c>
       <c r="R21" s="10"/>
       <c r="S21" s="10"/>
-      <c r="T21" s="10"/>
-      <c r="U21" s="10"/>
-      <c r="V21" s="10" t="s">
-        <v>39</v>
-      </c>
+      <c r="T21" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="U21" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="V21" s="10"/>
       <c r="W21" s="10"/>
       <c r="X21" s="10"/>
       <c r="Y21" s="10"/>
       <c r="Z21" s="10"/>
-    </row>
-    <row r="22" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="AA21" s="10"/>
+      <c r="AB21" s="10"/>
+      <c r="AC21" s="10"/>
+      <c r="AD21" s="10">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B22" s="5">
         <v>20</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D22" s="6">
-        <v>200048588</v>
+        <v>12</v>
+      </c>
+      <c r="D22" s="7">
+        <v>200135338</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F22" s="10"/>
       <c r="G22" s="10"/>
       <c r="H22" s="10"/>
       <c r="I22" s="10"/>
       <c r="J22" s="10"/>
-      <c r="K22" s="10" t="s">
-        <v>39</v>
-      </c>
+      <c r="K22" s="10"/>
       <c r="L22" s="10"/>
       <c r="M22" s="10"/>
       <c r="N22" s="10"/>
       <c r="O22" s="10"/>
-      <c r="P22" s="10"/>
+      <c r="P22" s="10" t="s">
+        <v>39</v>
+      </c>
       <c r="Q22" s="10"/>
       <c r="R22" s="10"/>
       <c r="S22" s="10"/>
       <c r="T22" s="10"/>
-      <c r="U22" s="10" t="s">
-        <v>39</v>
-      </c>
+      <c r="U22" s="10"/>
       <c r="V22" s="10" t="s">
         <v>39</v>
       </c>
       <c r="W22" s="10"/>
-      <c r="X22" s="10" t="s">
-        <v>39</v>
-      </c>
+      <c r="X22" s="10"/>
       <c r="Y22" s="10"/>
       <c r="Z22" s="10"/>
-    </row>
-    <row r="23" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="AA22" s="10"/>
+      <c r="AB22" s="10"/>
+      <c r="AC22" s="10"/>
+      <c r="AD22" s="10">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B23" s="5">
         <v>21</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>14</v>
+        <v>132</v>
       </c>
       <c r="D23" s="7">
-        <v>200082252</v>
+        <v>200137840</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>22</v>
+        <v>133</v>
       </c>
       <c r="F23" s="10"/>
       <c r="G23" s="10"/>
@@ -1891,9 +2142,7 @@
       <c r="M23" s="10"/>
       <c r="N23" s="10"/>
       <c r="O23" s="10"/>
-      <c r="P23" s="10" t="s">
-        <v>39</v>
-      </c>
+      <c r="P23" s="10"/>
       <c r="Q23" s="10"/>
       <c r="R23" s="10"/>
       <c r="S23" s="10"/>
@@ -1903,29 +2152,38 @@
       <c r="W23" s="10"/>
       <c r="X23" s="10"/>
       <c r="Y23" s="10"/>
-      <c r="Z23" s="10" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="24" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="Z23" s="10"/>
+      <c r="AA23" s="10"/>
+      <c r="AB23" s="10"/>
+      <c r="AC23" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD23" s="10">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B24" s="5">
         <v>22</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="D24" s="7">
-        <v>200108361</v>
+        <v>13</v>
+      </c>
+      <c r="D24" s="6">
+        <v>200048588</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>101</v>
+        <v>21</v>
       </c>
       <c r="F24" s="10"/>
       <c r="G24" s="10"/>
       <c r="H24" s="10"/>
       <c r="I24" s="10"/>
       <c r="J24" s="10"/>
-      <c r="K24" s="10"/>
+      <c r="K24" s="10" t="s">
+        <v>39</v>
+      </c>
       <c r="L24" s="10"/>
       <c r="M24" s="10"/>
       <c r="N24" s="10"/>
@@ -1935,68 +2193,84 @@
       <c r="R24" s="10"/>
       <c r="S24" s="10"/>
       <c r="T24" s="10"/>
-      <c r="U24" s="10"/>
+      <c r="U24" s="10" t="s">
+        <v>39</v>
+      </c>
       <c r="V24" s="10" t="s">
         <v>39</v>
       </c>
       <c r="W24" s="10"/>
-      <c r="X24" s="10"/>
+      <c r="X24" s="10" t="s">
+        <v>39</v>
+      </c>
       <c r="Y24" s="10"/>
       <c r="Z24" s="10"/>
-    </row>
-    <row r="25" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="AA24" s="10"/>
+      <c r="AB24" s="10"/>
+      <c r="AC24" s="10"/>
+      <c r="AD24" s="10">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B25" s="5">
         <v>23</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D25" s="7">
-        <v>200136002</v>
+        <v>200082252</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F25" s="10"/>
       <c r="G25" s="10"/>
       <c r="H25" s="10"/>
       <c r="I25" s="10"/>
       <c r="J25" s="10"/>
-      <c r="K25" s="10" t="s">
-        <v>39</v>
-      </c>
+      <c r="K25" s="10"/>
       <c r="L25" s="10"/>
       <c r="M25" s="10"/>
       <c r="N25" s="10"/>
       <c r="O25" s="10"/>
-      <c r="P25" s="10"/>
+      <c r="P25" s="10" t="s">
+        <v>39</v>
+      </c>
       <c r="Q25" s="10"/>
       <c r="R25" s="10"/>
       <c r="S25" s="10"/>
-      <c r="T25" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="U25" s="10" t="s">
-        <v>39</v>
-      </c>
+      <c r="T25" s="10"/>
+      <c r="U25" s="10"/>
       <c r="V25" s="10"/>
       <c r="W25" s="10"/>
       <c r="X25" s="10"/>
       <c r="Y25" s="10"/>
-      <c r="Z25" s="10"/>
-    </row>
-    <row r="26" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="Z25" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="AA25" s="10"/>
+      <c r="AB25" s="10"/>
+      <c r="AC25" s="10"/>
+      <c r="AD25" s="10">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B26" s="5">
         <v>24</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>16</v>
+        <v>97</v>
       </c>
       <c r="D26" s="7">
-        <v>200135574</v>
+        <v>200108361</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>24</v>
+        <v>101</v>
       </c>
       <c r="F26" s="10"/>
       <c r="G26" s="10"/>
@@ -2008,41 +2282,48 @@
       <c r="M26" s="10"/>
       <c r="N26" s="10"/>
       <c r="O26" s="10"/>
-      <c r="P26" s="10" t="s">
-        <v>39</v>
-      </c>
+      <c r="P26" s="10"/>
       <c r="Q26" s="10"/>
       <c r="R26" s="10"/>
       <c r="S26" s="10"/>
       <c r="T26" s="10"/>
-      <c r="U26" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="V26" s="10"/>
+      <c r="U26" s="10"/>
+      <c r="V26" s="10" t="s">
+        <v>39</v>
+      </c>
       <c r="W26" s="10"/>
       <c r="X26" s="10"/>
       <c r="Y26" s="10"/>
       <c r="Z26" s="10"/>
-    </row>
-    <row r="27" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="AA26" s="10"/>
+      <c r="AB26" s="10"/>
+      <c r="AC26" s="10"/>
+      <c r="AD26" s="10">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B27" s="5">
         <v>25</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>77</v>
+        <v>15</v>
       </c>
       <c r="D27" s="7">
-        <v>200108882</v>
+        <v>200136002</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>85</v>
+        <v>23</v>
       </c>
       <c r="F27" s="10"/>
       <c r="G27" s="10"/>
       <c r="H27" s="10"/>
       <c r="I27" s="10"/>
       <c r="J27" s="10"/>
-      <c r="K27" s="10"/>
+      <c r="K27" s="10" t="s">
+        <v>39</v>
+      </c>
       <c r="L27" s="10"/>
       <c r="M27" s="10"/>
       <c r="N27" s="10"/>
@@ -2062,19 +2343,26 @@
       <c r="X27" s="10"/>
       <c r="Y27" s="10"/>
       <c r="Z27" s="10"/>
-    </row>
-    <row r="28" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="AA27" s="10"/>
+      <c r="AB27" s="10"/>
+      <c r="AC27" s="10"/>
+      <c r="AD27" s="10">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B28" s="5">
         <v>26</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D28" s="6">
-        <v>200109296</v>
+        <v>16</v>
+      </c>
+      <c r="D28" s="7">
+        <v>200135574</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F28" s="10"/>
       <c r="G28" s="10"/>
@@ -2084,81 +2372,87 @@
       <c r="K28" s="10"/>
       <c r="L28" s="10"/>
       <c r="M28" s="10"/>
-      <c r="N28" s="10" t="s">
-        <v>39</v>
-      </c>
+      <c r="N28" s="10"/>
       <c r="O28" s="10"/>
-      <c r="P28" s="10"/>
+      <c r="P28" s="10" t="s">
+        <v>39</v>
+      </c>
       <c r="Q28" s="10"/>
       <c r="R28" s="10"/>
       <c r="S28" s="10"/>
-      <c r="T28" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="U28" s="10"/>
+      <c r="T28" s="10"/>
+      <c r="U28" s="10" t="s">
+        <v>39</v>
+      </c>
       <c r="V28" s="10"/>
       <c r="W28" s="10"/>
       <c r="X28" s="10"/>
       <c r="Y28" s="10"/>
       <c r="Z28" s="10"/>
-    </row>
-    <row r="29" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="AA28" s="10"/>
+      <c r="AB28" s="10"/>
+      <c r="AC28" s="10"/>
+      <c r="AD28" s="10">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B29" s="5">
         <v>27</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>18</v>
+        <v>123</v>
       </c>
       <c r="D29" s="7">
-        <v>200134170</v>
+        <v>200135112</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>26</v>
+        <v>124</v>
       </c>
       <c r="F29" s="10"/>
       <c r="G29" s="10"/>
       <c r="H29" s="10"/>
       <c r="I29" s="10"/>
-      <c r="J29" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="K29" s="10" t="s">
-        <v>39</v>
-      </c>
+      <c r="J29" s="10"/>
+      <c r="K29" s="10"/>
       <c r="L29" s="10"/>
       <c r="M29" s="10"/>
       <c r="N29" s="10"/>
       <c r="O29" s="10"/>
       <c r="P29" s="10"/>
-      <c r="Q29" s="10" t="s">
-        <v>39</v>
-      </c>
+      <c r="Q29" s="10"/>
       <c r="R29" s="10"/>
       <c r="S29" s="10"/>
       <c r="T29" s="10"/>
-      <c r="U29" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="V29" s="10" t="s">
-        <v>39</v>
-      </c>
+      <c r="U29" s="10"/>
+      <c r="V29" s="10"/>
       <c r="W29" s="10"/>
       <c r="X29" s="10"/>
       <c r="Y29" s="10"/>
       <c r="Z29" s="10"/>
-    </row>
-    <row r="30" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="AA29" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="AB29" s="10"/>
+      <c r="AC29" s="10"/>
+      <c r="AD29" s="10">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B30" s="5">
         <v>28</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>99</v>
+        <v>77</v>
       </c>
       <c r="D30" s="7">
-        <v>200134299</v>
+        <v>200108882</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>102</v>
+        <v>85</v>
       </c>
       <c r="F30" s="10"/>
       <c r="G30" s="10"/>
@@ -2174,40 +2468,49 @@
       <c r="Q30" s="10"/>
       <c r="R30" s="10"/>
       <c r="S30" s="10"/>
-      <c r="T30" s="10"/>
-      <c r="U30" s="10"/>
-      <c r="V30" s="10" t="s">
-        <v>39</v>
-      </c>
+      <c r="T30" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="U30" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="V30" s="10"/>
       <c r="W30" s="10"/>
       <c r="X30" s="10"/>
       <c r="Y30" s="10"/>
       <c r="Z30" s="10"/>
-    </row>
-    <row r="31" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="AA30" s="10"/>
+      <c r="AB30" s="10"/>
+      <c r="AC30" s="10"/>
+      <c r="AD30" s="10">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B31" s="5">
         <v>29</v>
       </c>
-      <c r="C31" s="8" t="s">
-        <v>19</v>
+      <c r="C31" s="7" t="s">
+        <v>17</v>
       </c>
       <c r="D31" s="6">
-        <v>200107036</v>
+        <v>200109296</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F31" s="10"/>
       <c r="G31" s="10"/>
       <c r="H31" s="10"/>
-      <c r="I31" s="10" t="s">
-        <v>39</v>
-      </c>
+      <c r="I31" s="10"/>
       <c r="J31" s="10"/>
       <c r="K31" s="10"/>
       <c r="L31" s="10"/>
       <c r="M31" s="10"/>
-      <c r="N31" s="10"/>
+      <c r="N31" s="10" t="s">
+        <v>39</v>
+      </c>
       <c r="O31" s="10"/>
       <c r="P31" s="10"/>
       <c r="Q31" s="10"/>
@@ -2222,47 +2525,222 @@
       <c r="X31" s="10"/>
       <c r="Y31" s="10"/>
       <c r="Z31" s="10"/>
-    </row>
-    <row r="32" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="AA31" s="10"/>
+      <c r="AB31" s="10"/>
+      <c r="AC31" s="10"/>
+      <c r="AD31" s="10">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B32" s="5">
         <v>30</v>
       </c>
-      <c r="C32" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="D32" s="6">
-        <v>200107506</v>
+      <c r="C32" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D32" s="7">
+        <v>200134170</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>86</v>
+        <v>26</v>
       </c>
       <c r="F32" s="10"/>
       <c r="G32" s="10"/>
       <c r="H32" s="10"/>
-      <c r="I32" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="J32" s="10"/>
-      <c r="K32" s="10"/>
+      <c r="I32" s="10"/>
+      <c r="J32" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="K32" s="10" t="s">
+        <v>39</v>
+      </c>
       <c r="L32" s="10"/>
       <c r="M32" s="10"/>
       <c r="N32" s="10"/>
       <c r="O32" s="10"/>
       <c r="P32" s="10"/>
-      <c r="Q32" s="10"/>
+      <c r="Q32" s="10" t="s">
+        <v>39</v>
+      </c>
       <c r="R32" s="10"/>
       <c r="S32" s="10"/>
-      <c r="T32" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="U32" s="10"/>
-      <c r="V32" s="10"/>
+      <c r="T32" s="10"/>
+      <c r="U32" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="V32" s="10" t="s">
+        <v>39</v>
+      </c>
       <c r="W32" s="10"/>
       <c r="X32" s="10"/>
       <c r="Y32" s="10"/>
       <c r="Z32" s="10"/>
+      <c r="AA32" s="10"/>
+      <c r="AB32" s="10"/>
+      <c r="AC32" s="10"/>
+      <c r="AD32" s="10">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="2:30" x14ac:dyDescent="0.3">
+      <c r="B33" s="5">
+        <v>31</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="D33" s="7">
+        <v>200134299</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="F33" s="10"/>
+      <c r="G33" s="10"/>
+      <c r="H33" s="10"/>
+      <c r="I33" s="10"/>
+      <c r="J33" s="10"/>
+      <c r="K33" s="10"/>
+      <c r="L33" s="10"/>
+      <c r="M33" s="10"/>
+      <c r="N33" s="10"/>
+      <c r="O33" s="10"/>
+      <c r="P33" s="10"/>
+      <c r="Q33" s="10"/>
+      <c r="R33" s="10"/>
+      <c r="S33" s="10"/>
+      <c r="T33" s="10"/>
+      <c r="U33" s="10"/>
+      <c r="V33" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="W33" s="10"/>
+      <c r="X33" s="10"/>
+      <c r="Y33" s="10"/>
+      <c r="Z33" s="10"/>
+      <c r="AA33" s="10"/>
+      <c r="AB33" s="10"/>
+      <c r="AC33" s="10"/>
+      <c r="AD33" s="10">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="2:30" x14ac:dyDescent="0.3">
+      <c r="B34" s="5">
+        <v>32</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D34" s="6">
+        <v>200107036</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F34" s="10"/>
+      <c r="G34" s="10"/>
+      <c r="H34" s="10"/>
+      <c r="I34" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="J34" s="10"/>
+      <c r="K34" s="10"/>
+      <c r="L34" s="10"/>
+      <c r="M34" s="10"/>
+      <c r="N34" s="10"/>
+      <c r="O34" s="10"/>
+      <c r="P34" s="10"/>
+      <c r="Q34" s="10"/>
+      <c r="R34" s="10"/>
+      <c r="S34" s="10"/>
+      <c r="T34" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="U34" s="10"/>
+      <c r="V34" s="10"/>
+      <c r="W34" s="10"/>
+      <c r="X34" s="10"/>
+      <c r="Y34" s="10"/>
+      <c r="Z34" s="10"/>
+      <c r="AA34" s="10"/>
+      <c r="AB34" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC34" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD34" s="10">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="2:30" x14ac:dyDescent="0.3">
+      <c r="B35" s="5">
+        <v>33</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="D35" s="6">
+        <v>200107506</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="F35" s="10"/>
+      <c r="G35" s="10"/>
+      <c r="H35" s="10"/>
+      <c r="I35" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="J35" s="10"/>
+      <c r="K35" s="10"/>
+      <c r="L35" s="10"/>
+      <c r="M35" s="10"/>
+      <c r="N35" s="10"/>
+      <c r="O35" s="10"/>
+      <c r="P35" s="10"/>
+      <c r="Q35" s="10"/>
+      <c r="R35" s="10"/>
+      <c r="S35" s="10"/>
+      <c r="T35" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="U35" s="10"/>
+      <c r="V35" s="10"/>
+      <c r="W35" s="10"/>
+      <c r="X35" s="10"/>
+      <c r="Y35" s="10"/>
+      <c r="Z35" s="10"/>
+      <c r="AA35" s="10"/>
+      <c r="AB35" s="10"/>
+      <c r="AC35" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD35" s="10">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="2:30" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AB36" s="24" t="s">
+        <v>131</v>
+      </c>
+      <c r="AC36" s="24"/>
+      <c r="AD36" s="25">
+        <f>SUM(AD3:AD35)</f>
+        <v>97</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="AB36:AC36"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
 </worksheet>
@@ -2270,10 +2748,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53390297-B1EB-4F05-BF18-BF0D31A69F5E}">
-  <dimension ref="B2:E23"/>
+  <dimension ref="B2:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2584,6 +3062,48 @@
         <v>116</v>
       </c>
     </row>
+    <row r="24" spans="2:5" ht="82.8" x14ac:dyDescent="0.3">
+      <c r="B24" s="15">
+        <v>44330</v>
+      </c>
+      <c r="C24" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="D24" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="E24" s="19" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" ht="69" x14ac:dyDescent="0.3">
+      <c r="B25" s="15">
+        <v>44337</v>
+      </c>
+      <c r="C25" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="D25" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="E25" s="19" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="B26" s="15">
+        <v>44338</v>
+      </c>
+      <c r="C26" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="D26" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="E26" s="20" t="s">
+        <v>125</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="14" type="noConversion"/>
   <hyperlinks>
@@ -2596,8 +3116,9 @@
     <hyperlink ref="E17" r:id="rId7" xr:uid="{65123D90-E02A-4775-9E7C-4354D603709B}"/>
     <hyperlink ref="E19" r:id="rId8" xr:uid="{BD699360-E531-49E4-8141-D5A0F3FF9101}"/>
     <hyperlink ref="E21" r:id="rId9" xr:uid="{571153F2-1E4B-41A8-B7EE-F9BA5380BBE6}"/>
+    <hyperlink ref="E26" r:id="rId10" xr:uid="{4A015FD2-CD6B-4A3F-ACD3-BB86B4908099}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="1200" r:id="rId10"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="1200" r:id="rId11"/>
 </worksheet>
 </file>
</xml_diff>